<commit_message>
Cuaderno de estudio MA_09_12_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion12/ESCALETA_ MA_09_12_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion12/ESCALETA_ MA_09_12_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16875" windowHeight="7215"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="160">
   <si>
     <t>Asignatura</t>
   </si>
@@ -211,9 +216,6 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Mapa conceptual: Estadistica</t>
-  </si>
-  <si>
     <t>Mapa conceptual sobre la estadistica</t>
   </si>
   <si>
@@ -244,12 +246,6 @@
     <t>El estudio estadístico. Población y muestra</t>
   </si>
   <si>
-    <t>Repasa concpetos básicos de estadística</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Analisis de variables</t>
-  </si>
-  <si>
     <t xml:space="preserve">Presentar en las imágenes la organización de datos en tablas agrupadas. Se indaga por el número de intervalos; por el tamaño o rango, por cierta clase, por la frecuencia absoluta de la clase seleccionada, por la frecuencia acumuklada relativa, etc. </t>
   </si>
   <si>
@@ -503,6 +499,12 @@
   </si>
   <si>
     <t>MTC_09_11</t>
+  </si>
+  <si>
+    <t>Mapa conceptual: La estadistica</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El análisis de variables</t>
   </si>
 </sst>
 </file>
@@ -938,6 +940,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -976,39 +1011,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,7 +1072,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1105,7 +1107,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1316,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GE161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1349,94 +1351,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="49" t="s">
+      <c r="D1" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="J1" s="58" t="s">
+      <c r="H1" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="63" t="s">
+      <c r="Q1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="63" t="s">
+      <c r="S1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="63" t="s">
+      <c r="U1" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="49"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="60"/>
       <c r="M2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="66"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="63"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="54"/>
     </row>
     <row r="3" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1446,15 +1448,15 @@
         <v>33</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E3" s="44"/>
       <c r="F3" s="14"/>
       <c r="G3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="16">
         <v>1</v>
@@ -1463,10 +1465,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>19</v>
@@ -1475,22 +1477,22 @@
       <c r="N3" s="21"/>
       <c r="O3" s="22"/>
       <c r="P3" s="23" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="Q3" s="24">
         <v>10</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T3" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U3" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,27 +1503,27 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E4" s="44"/>
       <c r="F4" s="14"/>
       <c r="G4" s="15" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="H4" s="16">
         <v>2</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L4" s="20" t="s">
         <v>21</v>
@@ -1530,22 +1532,22 @@
       <c r="N4" s="21"/>
       <c r="O4" s="22"/>
       <c r="P4" s="23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q4" s="24">
         <v>10</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T4" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="U4" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:187" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,17 +1558,17 @@
         <v>33</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -1575,10 +1577,10 @@
         <v>18</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L5" s="20" t="s">
         <v>19</v>
@@ -1588,7 +1590,7 @@
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P5" s="31" t="s">
         <v>18</v>
@@ -1600,13 +1602,13 @@
         <v>20</v>
       </c>
       <c r="S5" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="T5" s="70" t="s">
-        <v>136</v>
+        <v>132</v>
+      </c>
+      <c r="T5" s="49" t="s">
+        <v>133</v>
       </c>
       <c r="U5" s="32" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="EA5" s="4"/>
       <c r="EB5" s="4"/>
@@ -1674,17 +1676,17 @@
         <v>33</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="33"/>
       <c r="G6" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" s="16">
         <v>4</v>
@@ -1696,7 +1698,7 @@
         <v>37</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>21</v>
@@ -1706,7 +1708,7 @@
         <v>22</v>
       </c>
       <c r="O6" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P6" s="37" t="s">
         <v>18</v>
@@ -1718,13 +1720,13 @@
         <v>38</v>
       </c>
       <c r="S6" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T6" s="70" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="T6" s="49" t="s">
+        <v>137</v>
       </c>
       <c r="U6" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1735,17 +1737,17 @@
         <v>33</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="16">
         <v>5</v>
@@ -1757,7 +1759,7 @@
         <v>40</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L7" s="20" t="s">
         <v>21</v>
@@ -1767,7 +1769,7 @@
         <v>23</v>
       </c>
       <c r="O7" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P7" s="37" t="s">
         <v>18</v>
@@ -1779,13 +1781,13 @@
         <v>38</v>
       </c>
       <c r="S7" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T7" s="70" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="T7" s="49" t="s">
+        <v>140</v>
       </c>
       <c r="U7" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1796,10 +1798,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E8" s="46" t="s">
         <v>41</v>
@@ -1818,7 +1820,7 @@
         <v>43</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L8" s="20" t="s">
         <v>21</v>
@@ -1840,13 +1842,13 @@
         <v>38</v>
       </c>
       <c r="S8" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="T8" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="T8" s="70" t="s">
-        <v>142</v>
-      </c>
       <c r="U8" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1857,17 +1859,17 @@
         <v>33</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="34" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="H9" s="16">
         <v>7</v>
@@ -1876,10 +1878,10 @@
         <v>36</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L9" s="20" t="s">
         <v>21</v>
@@ -1901,13 +1903,13 @@
         <v>38</v>
       </c>
       <c r="S9" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T9" s="70" t="s">
-        <v>151</v>
+        <v>136</v>
+      </c>
+      <c r="T9" s="49" t="s">
+        <v>148</v>
       </c>
       <c r="U9" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:187" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,27 +1920,27 @@
         <v>33</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="33"/>
       <c r="G10" s="34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L10" s="20" t="s">
         <v>19</v>
@@ -1953,16 +1955,16 @@
         <v>10</v>
       </c>
       <c r="R10" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S10" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T10" s="71" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="T10" s="50" t="s">
+        <v>111</v>
       </c>
       <c r="U10" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,17 +1975,17 @@
         <v>33</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H11" s="16">
         <v>9</v>
@@ -1995,7 +1997,7 @@
         <v>48</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L11" s="20" t="s">
         <v>21</v>
@@ -2005,7 +2007,7 @@
         <v>23</v>
       </c>
       <c r="O11" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P11" s="37" t="s">
         <v>18</v>
@@ -2017,13 +2019,13 @@
         <v>38</v>
       </c>
       <c r="S11" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T11" s="70" t="s">
-        <v>144</v>
+        <v>136</v>
+      </c>
+      <c r="T11" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="U11" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:187" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2034,10 +2036,10 @@
         <v>33</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>45</v>
@@ -2053,10 +2055,10 @@
         <v>36</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L12" s="20" t="s">
         <v>21</v>
@@ -2073,16 +2075,16 @@
         <v>10</v>
       </c>
       <c r="R12" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S12" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T12" s="71" t="s">
-        <v>121</v>
+        <v>98</v>
+      </c>
+      <c r="T12" s="50" t="s">
+        <v>118</v>
       </c>
       <c r="U12" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:187" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,7 +2095,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>51</v>
@@ -2101,7 +2103,7 @@
       <c r="E13" s="46"/>
       <c r="F13" s="33"/>
       <c r="G13" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H13" s="16">
         <v>11</v>
@@ -2110,10 +2112,10 @@
         <v>36</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L13" s="20" t="s">
         <v>21</v>
@@ -2122,22 +2124,22 @@
       <c r="N13" s="29"/>
       <c r="O13" s="36"/>
       <c r="P13" s="37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q13" s="32">
         <v>8</v>
       </c>
       <c r="R13" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S13" s="32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="T13" s="32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U13" s="32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -2314,7 +2316,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>51</v>
@@ -2322,7 +2324,7 @@
       <c r="E14" s="46"/>
       <c r="F14" s="33"/>
       <c r="G14" s="34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H14" s="16">
         <v>12</v>
@@ -2331,10 +2333,10 @@
         <v>36</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L14" s="20" t="s">
         <v>21</v>
@@ -2344,10 +2346,10 @@
         <v>26</v>
       </c>
       <c r="O14" s="36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P14" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q14" s="32">
         <v>6</v>
@@ -2356,13 +2358,13 @@
         <v>38</v>
       </c>
       <c r="S14" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T14" s="70" t="s">
-        <v>145</v>
+        <v>136</v>
+      </c>
+      <c r="T14" s="49" t="s">
+        <v>142</v>
       </c>
       <c r="U14" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2373,7 +2375,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>51</v>
@@ -2381,7 +2383,7 @@
       <c r="E15" s="46"/>
       <c r="F15" s="33"/>
       <c r="G15" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H15" s="16">
         <v>13</v>
@@ -2390,10 +2392,10 @@
         <v>18</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L15" s="20" t="s">
         <v>19</v>
@@ -2402,22 +2404,22 @@
       <c r="N15" s="29"/>
       <c r="O15" s="36"/>
       <c r="P15" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="32">
         <v>10</v>
       </c>
       <c r="R15" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S15" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T15" s="71" t="s">
-        <v>80</v>
+        <v>98</v>
+      </c>
+      <c r="T15" s="50" t="s">
+        <v>77</v>
       </c>
       <c r="U15" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:187" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2430,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>51</v>
@@ -2447,10 +2449,10 @@
         <v>18</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L16" s="20" t="s">
         <v>19</v>
@@ -2458,25 +2460,25 @@
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P16" s="37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q16">
         <v>9</v>
       </c>
       <c r="R16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T16" t="s">
         <v>53</v>
       </c>
       <c r="U16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2487,7 +2489,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>51</v>
@@ -2495,19 +2497,19 @@
       <c r="E17" s="46"/>
       <c r="F17" s="33"/>
       <c r="G17" s="34" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H17" s="16">
         <v>15</v>
       </c>
       <c r="I17" s="35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L17" s="20" t="s">
         <v>21</v>
@@ -2516,22 +2518,22 @@
       <c r="N17" s="29"/>
       <c r="O17" s="36"/>
       <c r="P17" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q17" s="32">
         <v>10</v>
       </c>
       <c r="R17" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S17" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T17" s="71" t="s">
-        <v>116</v>
+        <v>98</v>
+      </c>
+      <c r="T17" s="50" t="s">
+        <v>113</v>
       </c>
       <c r="U17" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2544,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>51</v>
@@ -2564,7 +2566,7 @@
         <v>56</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L18" s="20" t="s">
         <v>21</v>
@@ -2572,7 +2574,7 @@
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P18" s="37" t="s">
         <v>18</v>
@@ -2581,16 +2583,16 @@
         <v>10</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S18" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T18" s="71" t="s">
-        <v>122</v>
+        <v>98</v>
+      </c>
+      <c r="T18" s="50" t="s">
+        <v>119</v>
       </c>
       <c r="U18" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2601,7 +2603,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>54</v>
@@ -2618,10 +2620,10 @@
         <v>18</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L19" s="20" t="s">
         <v>19</v>
@@ -2631,10 +2633,10 @@
       </c>
       <c r="N19" s="29"/>
       <c r="O19" s="36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P19" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q19" s="32">
         <v>6</v>
@@ -2643,13 +2645,13 @@
         <v>20</v>
       </c>
       <c r="S19" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="T19" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="T19" s="70" t="s">
-        <v>138</v>
-      </c>
       <c r="U19" s="32" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2660,7 +2662,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>54</v>
@@ -2670,7 +2672,7 @@
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H20" s="16">
         <v>18</v>
@@ -2679,10 +2681,10 @@
         <v>36</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L20" s="20" t="s">
         <v>21</v>
@@ -2692,7 +2694,7 @@
         <v>32</v>
       </c>
       <c r="O20" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="P20" s="37" t="s">
         <v>18</v>
@@ -2704,13 +2706,13 @@
         <v>38</v>
       </c>
       <c r="S20" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="T20" s="70" t="s">
-        <v>148</v>
+        <v>144</v>
+      </c>
+      <c r="T20" s="49" t="s">
+        <v>145</v>
       </c>
       <c r="U20" s="32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2721,7 +2723,7 @@
         <v>33</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>54</v>
@@ -2731,7 +2733,7 @@
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="34" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H21" s="16">
         <v>19</v>
@@ -2743,7 +2745,7 @@
         <v>61</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>21</v>
@@ -2758,16 +2760,16 @@
         <v>9</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T21" s="71" t="s">
-        <v>153</v>
+        <v>98</v>
+      </c>
+      <c r="T21" s="50" t="s">
+        <v>150</v>
       </c>
       <c r="U21" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2778,7 +2780,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>54</v>
@@ -2786,7 +2788,7 @@
       <c r="E22" s="46"/>
       <c r="F22" s="33"/>
       <c r="G22" s="34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -2795,10 +2797,10 @@
         <v>36</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L22" s="20" t="s">
         <v>21</v>
@@ -2807,22 +2809,22 @@
       <c r="N22" s="29"/>
       <c r="O22" s="36"/>
       <c r="P22" s="37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q22" s="32">
         <v>10</v>
       </c>
       <c r="R22" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S22" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T22" s="71" t="s">
-        <v>123</v>
+        <v>98</v>
+      </c>
+      <c r="T22" s="50" t="s">
+        <v>120</v>
       </c>
       <c r="U22" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2833,7 +2835,7 @@
         <v>33</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>54</v>
@@ -2855,7 +2857,7 @@
         <v>59</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L23" s="20" t="s">
         <v>21</v>
@@ -2872,16 +2874,16 @@
         <v>10</v>
       </c>
       <c r="R23" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S23" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T23" s="71" t="s">
-        <v>124</v>
+        <v>98</v>
+      </c>
+      <c r="T23" s="50" t="s">
+        <v>121</v>
       </c>
       <c r="U23" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2892,15 +2894,15 @@
         <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E24" s="46"/>
       <c r="F24" s="33"/>
       <c r="G24" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H24" s="16">
         <v>22</v>
@@ -2909,10 +2911,10 @@
         <v>36</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L24" s="20" t="s">
         <v>21</v>
@@ -2921,22 +2923,22 @@
       <c r="N24" s="29"/>
       <c r="O24" s="36"/>
       <c r="P24" s="37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q24" s="32">
         <v>10</v>
       </c>
       <c r="R24" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S24" s="32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T24" s="32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U24" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2947,17 +2949,17 @@
         <v>33</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E25" s="46" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H25" s="16">
         <v>23</v>
@@ -2966,10 +2968,10 @@
         <v>36</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L25" s="20" t="s">
         <v>21</v>
@@ -2984,16 +2986,16 @@
         <v>10</v>
       </c>
       <c r="R25" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S25" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="T25" s="71" t="s">
-        <v>126</v>
+        <v>98</v>
+      </c>
+      <c r="T25" s="50" t="s">
+        <v>123</v>
       </c>
       <c r="U25" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3004,17 +3006,17 @@
         <v>33</v>
       </c>
       <c r="C26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="42" t="s">
-        <v>104</v>
-      </c>
       <c r="E26" s="46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H26" s="16">
         <v>24</v>
@@ -3023,10 +3025,10 @@
         <v>36</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L26" s="20" t="s">
         <v>21</v>
@@ -3036,7 +3038,7 @@
         <v>24</v>
       </c>
       <c r="O26" s="36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="P26" s="37" t="s">
         <v>18</v>
@@ -3048,13 +3050,13 @@
         <v>38</v>
       </c>
       <c r="S26" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T26" s="70" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="T26" s="49" t="s">
+        <v>143</v>
       </c>
       <c r="U26" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3065,17 +3067,17 @@
         <v>33</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="34" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="H27" s="16">
         <v>25</v>
@@ -3084,10 +3086,10 @@
         <v>36</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L27" s="20" t="s">
         <v>28</v>
@@ -3101,7 +3103,7 @@
       <c r="Q27" s="40"/>
       <c r="R27" s="41"/>
       <c r="S27" s="41"/>
-      <c r="T27" s="72"/>
+      <c r="T27" s="51"/>
       <c r="U27" s="41"/>
     </row>
     <row r="28" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3112,17 +3114,17 @@
         <v>33</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E28" s="46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F28" s="33"/>
       <c r="G28" s="34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3131,10 +3133,10 @@
         <v>36</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L28" s="20" t="s">
         <v>21</v>
@@ -3144,7 +3146,7 @@
         <v>22</v>
       </c>
       <c r="O28" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P28" s="37" t="s">
         <v>62</v>
@@ -3156,13 +3158,13 @@
         <v>38</v>
       </c>
       <c r="S28" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="T28" s="70" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="T28" s="49" t="s">
+        <v>137</v>
       </c>
       <c r="U28" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3173,17 +3175,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F29" s="33"/>
       <c r="G29" s="34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H29" s="16">
         <v>27</v>
@@ -3192,10 +3194,10 @@
         <v>36</v>
       </c>
       <c r="J29" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="K29" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="L29" s="20" t="s">
         <v>21</v>
@@ -3206,7 +3208,7 @@
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="43" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q29">
         <v>6</v>
@@ -3215,13 +3217,13 @@
         <v>38</v>
       </c>
       <c r="S29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="T29" s="48" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="U29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5443,14 +5445,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -5463,6 +5457,14 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A29">

</xml_diff>